<commit_message>
Correções e sugestões no modelo de casos de uso.
</commit_message>
<xml_diff>
--- a/Lista Inicial de Requisitos.xlsx
+++ b/Lista Inicial de Requisitos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>NUM</t>
   </si>
@@ -185,13 +185,34 @@
   </si>
   <si>
     <t>UC12</t>
+  </si>
+  <si>
+    <t>No Diagrama de UC é Cadastrar Funcionário</t>
+  </si>
+  <si>
+    <t>No Diagrama de UC é Manter Funcionários</t>
+  </si>
+  <si>
+    <t>No Diagrama, o Gerente está sem acesso a este UC</t>
+  </si>
+  <si>
+    <t>Deveria haver somente um UC de Login</t>
+  </si>
+  <si>
+    <t>Não vejo razão para este UC, me parece que a seleção do boleto é apenas um passo do UC de fazer o "upload" dos boletos.</t>
+  </si>
+  <si>
+    <t>Fazer Upload de Boletos é um nome melhor, usar verbo no infinitivo.</t>
+  </si>
+  <si>
+    <t>Ainda não entendi bem o que significa esse Upload. Se os boletos já estão em uma pasta do sistema, está sendo feito upload para onde? Parece que os arquivos já existem em algum lugar e apenas estão sendo renomeados. Falta esclarecer melhor essa questão.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -271,11 +292,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -302,6 +343,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,7 +445,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -427,7 +479,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -603,22 +654,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="32.5703125" customWidth="1"/>
+    <col min="6" max="6" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -635,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="5" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
@@ -651,8 +703,11 @@
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -668,8 +723,11 @@
       <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -685,8 +743,11 @@
       <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -702,8 +763,11 @@
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F6" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -719,8 +783,11 @@
       <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F7" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -736,8 +803,11 @@
       <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F8" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -755,7 +825,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="45">
       <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
@@ -771,9 +841,11 @@
       <c r="E10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75">
       <c r="A11" s="6" t="s">
         <v>35</v>
       </c>
@@ -783,9 +855,11 @@
       <c r="C11" s="8"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F11" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="6" t="s">
         <v>36</v>
       </c>
@@ -801,9 +875,11 @@
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="6" t="s">
         <v>37</v>
       </c>
@@ -821,7 +897,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="6" t="s">
         <v>38</v>
       </c>
@@ -839,7 +915,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="6" t="s">
         <v>39</v>
       </c>
@@ -857,7 +933,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -865,7 +941,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -873,7 +949,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -881,7 +957,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -889,7 +965,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -897,7 +973,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="B25" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sistema Atualizado + especificaçao UC05
Sistema Calendário revisado, corrigido e incluido a especificaçao do
UC05 para análise do professor.
</commit_message>
<xml_diff>
--- a/Lista Inicial de Requisitos.xlsx
+++ b/Lista Inicial de Requisitos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>NUM</t>
   </si>
@@ -46,33 +46,18 @@
     <t>Manter Clientes</t>
   </si>
   <si>
-    <t>Manter Usuários</t>
-  </si>
-  <si>
     <t>Manter cadastro dos clientes do escritório</t>
   </si>
   <si>
     <t>Consultar Agenda de Vencimentos</t>
   </si>
   <si>
-    <t>Fazer Login Cliente</t>
-  </si>
-  <si>
-    <t>Fazer Login Funcionário</t>
-  </si>
-  <si>
-    <t>Cadastrar usuário</t>
-  </si>
-  <si>
     <t>Cadastrar cliente</t>
   </si>
   <si>
     <t>O funcionário possui um login para cessar o sistema</t>
   </si>
   <si>
-    <t>Para fazer o Upload dos boletos o funcionário aponta a pasta que contém estes através do sistema</t>
-  </si>
-  <si>
     <t>O funcionário pode consultar o histórico dos boletos enviados</t>
   </si>
   <si>
@@ -133,15 +118,9 @@
     <t>RE12</t>
   </si>
   <si>
-    <t>RE13</t>
-  </si>
-  <si>
     <t>UC01</t>
   </si>
   <si>
-    <t>Cadastrar Usuário</t>
-  </si>
-  <si>
     <t>UC02</t>
   </si>
   <si>
@@ -160,9 +139,6 @@
     <t>UC07</t>
   </si>
   <si>
-    <t>Upload de Boletos</t>
-  </si>
-  <si>
     <t>UC08</t>
   </si>
   <si>
@@ -178,41 +154,29 @@
     <t>UC10</t>
   </si>
   <si>
-    <t>UC11</t>
-  </si>
-  <si>
-    <t>Selecionar Boletos</t>
-  </si>
-  <si>
-    <t>UC12</t>
-  </si>
-  <si>
-    <t>No Diagrama de UC é Cadastrar Funcionário</t>
-  </si>
-  <si>
-    <t>No Diagrama de UC é Manter Funcionários</t>
-  </si>
-  <si>
-    <t>No Diagrama, o Gerente está sem acesso a este UC</t>
-  </si>
-  <si>
-    <t>Deveria haver somente um UC de Login</t>
-  </si>
-  <si>
-    <t>Não vejo razão para este UC, me parece que a seleção do boleto é apenas um passo do UC de fazer o "upload" dos boletos.</t>
-  </si>
-  <si>
-    <t>Fazer Upload de Boletos é um nome melhor, usar verbo no infinitivo.</t>
-  </si>
-  <si>
-    <t>Ainda não entendi bem o que significa esse Upload. Se os boletos já estão em uma pasta do sistema, está sendo feito upload para onde? Parece que os arquivos já existem em algum lugar e apenas estão sendo renomeados. Falta esclarecer melhor essa questão.</t>
+    <t>Cadastrar Funcionario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazer Login </t>
+  </si>
+  <si>
+    <t>Fazer Login</t>
+  </si>
+  <si>
+    <t>Cadastrar Funcionário</t>
+  </si>
+  <si>
+    <t>Manter Funcionário</t>
+  </si>
+  <si>
+    <t>Enviar Boletos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +296,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -343,18 +319,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,6 +409,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -479,6 +444,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -654,14 +620,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
@@ -670,7 +636,7 @@
     <col min="6" max="6" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -687,75 +653,69 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1">
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -763,224 +723,154 @@
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30">
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="45">
+      <c r="E9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="75">
-      <c r="A11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30">
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
-      <c r="A15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="B25" s="3"/>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização - etapa 2
inclusão do DSS UC05
</commit_message>
<xml_diff>
--- a/Lista Inicial de Requisitos.xlsx
+++ b/Lista Inicial de Requisitos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>NUM</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>Sistema</t>
-  </si>
-  <si>
     <t>Manter Clientes</t>
   </si>
   <si>
@@ -170,16 +167,13 @@
   </si>
   <si>
     <t>O cliente possui um login para acessar o sistema</t>
-  </si>
-  <si>
-    <t>Não entendi porque o Sistema participaria deste UC se na descrição se afirma que é o funcionário que entra no sistema para enviar os boletos. Neste caso então o ator seria o funcionário e não o sistema. O sistema só seria ator se o UC fosse executado sem intervenção humana.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +406,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -446,6 +441,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -621,14 +617,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
@@ -637,7 +633,7 @@
     <col min="6" max="6" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -654,191 +650,189 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1">
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="75">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45">
-      <c r="A10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="30">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>3</v>
@@ -848,25 +842,25 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="30">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
     </row>
   </sheetData>

</xml_diff>